<commit_message>
Reorganized static files and put data into knowledge repo. About to get wild with styling.
</commit_message>
<xml_diff>
--- a/MySite/blog/static/websiteDB.xlsx
+++ b/MySite/blog/static/websiteDB.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15314\source\repos\MySite\MySite\blog\static\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\users\15314\source\repos\mysite\mysite\blog\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E31C8E1-A3AF-4142-83D5-655FEE32FFD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7658ECD6-80A7-4CC9-A9F3-774CDCB478FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3756" yWindow="2880" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{E658BFBE-975E-47B3-8C51-826238D4C145}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{E658BFBE-975E-47B3-8C51-826238D4C145}"/>
   </bookViews>
   <sheets>
     <sheet name="Posts" sheetId="4" r:id="rId1"/>
@@ -982,9 +982,6 @@
     <t>https://fred.stlouisfed.org/</t>
   </si>
   <si>
-    <t>Finance;Data</t>
-  </si>
-  <si>
     <t>Oshaughnessy Asset Management</t>
   </si>
   <si>
@@ -1003,9 +1000,6 @@
     <t>https://treasurydirect.gov/govt/reports/pd/histdebt/histdebt_histo5.htm</t>
   </si>
   <si>
-    <t>Finance;Debt;Government</t>
-  </si>
-  <si>
     <t>Al Sweigart</t>
   </si>
   <si>
@@ -1015,9 +1009,6 @@
     <t>https://automatetheboringstuff.com/</t>
   </si>
   <si>
-    <t>Programming;Python</t>
-  </si>
-  <si>
     <t>W3Schools</t>
   </si>
   <si>
@@ -1063,18 +1054,12 @@
     <t>https://alphaarchitect.com/blog/</t>
   </si>
   <si>
-    <t>Finance;Quanitative</t>
-  </si>
-  <si>
     <t>U.S Government's Financial Report</t>
   </si>
   <si>
     <t>https://fiscal.treasury.gov/reports-statements/financial-report/</t>
   </si>
   <si>
-    <t>Finance;Government</t>
-  </si>
-  <si>
     <t>John Geanakoplos</t>
   </si>
   <si>
@@ -1090,9 +1075,6 @@
     <t>http://aswathdamodaran.blogspot.com/</t>
   </si>
   <si>
-    <t>Finance;Blog</t>
-  </si>
-  <si>
     <t>Josh Brown</t>
   </si>
   <si>
@@ -1189,9 +1171,6 @@
     <t>https://archive.ics.uci.edu/ml/index.php</t>
   </si>
   <si>
-    <t>Programming;Data</t>
-  </si>
-  <si>
     <t>Learn Razor Pages</t>
   </si>
   <si>
@@ -1201,9 +1180,6 @@
     <t>https://www.learnrazorpages.com/</t>
   </si>
   <si>
-    <t>Programming;C#;Web Development</t>
-  </si>
-  <si>
     <t>Kudvenkat</t>
   </si>
   <si>
@@ -1222,9 +1198,6 @@
     <t>https://www.youtube.com/channel/UC-ptWR16ITQyYOglXyQmpzw</t>
   </si>
   <si>
-    <t>Programming; C#</t>
-  </si>
-  <si>
     <t>Bootstrap</t>
   </si>
   <si>
@@ -1234,9 +1207,6 @@
     <t>https://getbootstrap.com/</t>
   </si>
   <si>
-    <t>Programming; Web Development</t>
-  </si>
-  <si>
     <t>Beautiful Soup</t>
   </si>
   <si>
@@ -1246,9 +1216,6 @@
     <t>https://www.crummy.com/software/BeautifulSoup/bs4/doc/</t>
   </si>
   <si>
-    <t>Programming;Data;Python</t>
-  </si>
-  <si>
     <t>Phil Leggetter</t>
   </si>
   <si>
@@ -1258,9 +1225,6 @@
     <t>https://www.smashingmagazine.com/2012/05/building-real-time-commenting-system/</t>
   </si>
   <si>
-    <t>HTML;CSS; Web Development</t>
-  </si>
-  <si>
     <t>David Rubenstein</t>
   </si>
   <si>
@@ -1279,9 +1243,6 @@
     <t>https://riptutorial.com/epplus</t>
   </si>
   <si>
-    <t>C#;Programming;Excel;EPPlus</t>
-  </si>
-  <si>
     <t>xlWing</t>
   </si>
   <si>
@@ -1291,9 +1252,6 @@
     <t>https://docs.xlwings.org/en/stable/index.html</t>
   </si>
   <si>
-    <t>Python; Programming; Excel</t>
-  </si>
-  <si>
     <t>Okta Developer Platform</t>
   </si>
   <si>
@@ -1301,9 +1259,6 @@
   </si>
   <si>
     <t>https://developer.okta.com/blog/2020/01/02/mongodb-csharp-aspnet-datastore</t>
-  </si>
-  <si>
-    <t>Programming; Database; MongoDB</t>
   </si>
   <si>
     <t>Jan Kallman</t>
@@ -1637,9 +1592,6 @@
   </si>
   <si>
     <t>C# and Python tutorials. Has good guides for LINQ in C#</t>
-  </si>
-  <si>
-    <t>C#;Programming;Python;LINQ</t>
   </si>
   <si>
     <t>I used this sub/function combo to apply the named ranges in a selected range in excel. So it changes all formula references to excel cells to references to named ranges if they are applicable. I do remember having a lot of difficulty working with named ranges in vba so hopefully it still works and doesn't cause trouble.</t>
@@ -1771,9 +1723,6 @@
     <t>https://www.pygame.org/docs/</t>
   </si>
   <si>
-    <t>Python; Programming; Pygame;</t>
-  </si>
-  <si>
     <t>Documentation and tutorials for using python's Pygame library</t>
   </si>
   <si>
@@ -1783,9 +1732,6 @@
     <t>https://mortada.net/python-api-for-fred.html</t>
   </si>
   <si>
-    <t>Python; Programming; FRED</t>
-  </si>
-  <si>
     <t>Mortada</t>
   </si>
   <si>
@@ -1795,9 +1741,6 @@
     <t>https://web.stanford.edu/group/csp/cs21/htmlcheatsheet.pdf</t>
   </si>
   <si>
-    <t>HTML;Web Development</t>
-  </si>
-  <si>
     <t>HTML Cheatsheet</t>
   </si>
   <si>
@@ -1810,9 +1753,6 @@
     <t>CSS CheatSheet</t>
   </si>
   <si>
-    <t>CSS;Web Development</t>
-  </si>
-  <si>
     <t>https://ehmatthes.github.io/pcc_2e/cheat_sheets/cheat_sheets/</t>
   </si>
   <si>
@@ -1820,9 +1760,6 @@
   </si>
   <si>
     <t>Python Cheatsheets</t>
-  </si>
-  <si>
-    <t>Python; Programming</t>
   </si>
   <si>
     <t>https://inventwithpython.com/hackingciphers.pdf</t>
@@ -1932,9 +1869,6 @@
     <t>https://pythex.org/</t>
   </si>
   <si>
-    <t>Python; Regex</t>
-  </si>
-  <si>
     <t>Helper tool for using and learning regex</t>
   </si>
   <si>
@@ -1950,9 +1884,6 @@
     <t>https://www.english-corpora.org/coca/</t>
   </si>
   <si>
-    <t>NLP; Language</t>
-  </si>
-  <si>
     <t>https://realpython.com/</t>
   </si>
   <si>
@@ -1971,9 +1902,6 @@
     <t>http://holoviews.org/reference/index.html</t>
   </si>
   <si>
-    <t>Python; Data; Visualization</t>
-  </si>
-  <si>
     <t>PageSpeed Insights</t>
   </si>
   <si>
@@ -1995,9 +1923,6 @@
     <t>https://pep8.org/</t>
   </si>
   <si>
-    <t>Python; programming</t>
-  </si>
-  <si>
     <t>Koyfin</t>
   </si>
   <si>
@@ -2005,9 +1930,6 @@
   </si>
   <si>
     <t>https://www.koyfin.com/research/</t>
-  </si>
-  <si>
-    <t>Finance; blog; research</t>
   </si>
   <si>
     <t>The following are notes I made while reading the book "More than You Know: finding Financials Wisdom in Unconventional Places" by Michael Mauboussin:
@@ -2309,6 +2231,84 @@
   </si>
   <si>
     <t>TheWolfofWallStreet (TheWolfofWallStreet1)</t>
+  </si>
+  <si>
+    <t>Finance,Data</t>
+  </si>
+  <si>
+    <t>Finance,Debt,Government</t>
+  </si>
+  <si>
+    <t>Programming,Python</t>
+  </si>
+  <si>
+    <t>Finance,Quanitative</t>
+  </si>
+  <si>
+    <t>Finance,Government</t>
+  </si>
+  <si>
+    <t>Finance,Blog</t>
+  </si>
+  <si>
+    <t>Programming,Data</t>
+  </si>
+  <si>
+    <t>Programming,C#,Web Development</t>
+  </si>
+  <si>
+    <t>Programming, C#</t>
+  </si>
+  <si>
+    <t>Programming, Web Development</t>
+  </si>
+  <si>
+    <t>Programming,Data,Python</t>
+  </si>
+  <si>
+    <t>HTML,CSS, Web Development</t>
+  </si>
+  <si>
+    <t>C#,Programming,Excel,EPPlus</t>
+  </si>
+  <si>
+    <t>Python, Programming, Excel</t>
+  </si>
+  <si>
+    <t>Programming, Database, MongoDB</t>
+  </si>
+  <si>
+    <t>C#,Programming,Python,LINQ</t>
+  </si>
+  <si>
+    <t>Python, Programming, Pygame,</t>
+  </si>
+  <si>
+    <t>Python, Programming, FRED</t>
+  </si>
+  <si>
+    <t>HTML,Web Development</t>
+  </si>
+  <si>
+    <t>CSS,Web Development</t>
+  </si>
+  <si>
+    <t>Python, Programming</t>
+  </si>
+  <si>
+    <t>Python, Regex</t>
+  </si>
+  <si>
+    <t>NLP, Language</t>
+  </si>
+  <si>
+    <t>Python, Data, Visualization</t>
+  </si>
+  <si>
+    <t>Python, programming</t>
+  </si>
+  <si>
+    <t>Finance, blog, research</t>
   </si>
 </sst>
 </file>
@@ -2712,7 +2712,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>425</v>
+        <v>410</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -3450,25 +3450,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>557</v>
+        <v>531</v>
       </c>
       <c r="B1" t="s">
-        <v>426</v>
+        <v>411</v>
       </c>
       <c r="C1" t="s">
-        <v>427</v>
+        <v>412</v>
       </c>
       <c r="D1" t="s">
-        <v>428</v>
+        <v>413</v>
       </c>
       <c r="E1" t="s">
-        <v>429</v>
+        <v>414</v>
       </c>
       <c r="F1" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="G1" t="s">
-        <v>559</v>
+        <v>533</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -3479,7 +3479,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>558</v>
+        <v>532</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -3491,7 +3491,7 @@
         <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>560</v>
+        <v>534</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -3514,7 +3514,7 @@
         <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>561</v>
+        <v>535</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -3537,7 +3537,7 @@
         <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>562</v>
+        <v>536</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -3560,7 +3560,7 @@
         <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>563</v>
+        <v>537</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -3583,7 +3583,7 @@
         <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>564</v>
+        <v>538</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -3606,7 +3606,7 @@
         <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>565</v>
+        <v>539</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -3629,7 +3629,7 @@
         <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>566</v>
+        <v>540</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -3652,7 +3652,7 @@
         <v>3</v>
       </c>
       <c r="G9" t="s">
-        <v>567</v>
+        <v>541</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -3675,7 +3675,7 @@
         <v>3</v>
       </c>
       <c r="G10" t="s">
-        <v>568</v>
+        <v>542</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -3698,7 +3698,7 @@
         <v>3</v>
       </c>
       <c r="G11" t="s">
-        <v>569</v>
+        <v>543</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -3721,7 +3721,7 @@
         <v>3</v>
       </c>
       <c r="G12" t="s">
-        <v>570</v>
+        <v>544</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -3744,7 +3744,7 @@
         <v>3</v>
       </c>
       <c r="G13" t="s">
-        <v>571</v>
+        <v>545</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -3767,7 +3767,7 @@
         <v>3</v>
       </c>
       <c r="G14" t="s">
-        <v>572</v>
+        <v>546</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -3790,7 +3790,7 @@
         <v>3</v>
       </c>
       <c r="G15" t="s">
-        <v>573</v>
+        <v>547</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -3813,7 +3813,7 @@
         <v>3</v>
       </c>
       <c r="G16" t="s">
-        <v>574</v>
+        <v>548</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -3836,7 +3836,7 @@
         <v>3</v>
       </c>
       <c r="G17" t="s">
-        <v>575</v>
+        <v>549</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -3859,7 +3859,7 @@
         <v>3</v>
       </c>
       <c r="G18" t="s">
-        <v>576</v>
+        <v>550</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -3882,7 +3882,7 @@
         <v>3</v>
       </c>
       <c r="G19" t="s">
-        <v>577</v>
+        <v>551</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -3905,7 +3905,7 @@
         <v>3</v>
       </c>
       <c r="G20" t="s">
-        <v>578</v>
+        <v>552</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -3928,7 +3928,7 @@
         <v>3</v>
       </c>
       <c r="G21" t="s">
-        <v>579</v>
+        <v>553</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -3951,7 +3951,7 @@
         <v>3</v>
       </c>
       <c r="G22" t="s">
-        <v>580</v>
+        <v>554</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -3974,7 +3974,7 @@
         <v>3</v>
       </c>
       <c r="G23" t="s">
-        <v>581</v>
+        <v>555</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -3997,7 +3997,7 @@
         <v>3</v>
       </c>
       <c r="G24" t="s">
-        <v>582</v>
+        <v>556</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -4020,7 +4020,7 @@
         <v>3</v>
       </c>
       <c r="G25" t="s">
-        <v>583</v>
+        <v>557</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -4043,7 +4043,7 @@
         <v>3</v>
       </c>
       <c r="G26" t="s">
-        <v>584</v>
+        <v>558</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -4066,7 +4066,7 @@
         <v>3</v>
       </c>
       <c r="G27" t="s">
-        <v>585</v>
+        <v>559</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -4089,7 +4089,7 @@
         <v>3</v>
       </c>
       <c r="G28" t="s">
-        <v>586</v>
+        <v>560</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -4112,7 +4112,7 @@
         <v>3</v>
       </c>
       <c r="G29" t="s">
-        <v>587</v>
+        <v>561</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -4135,7 +4135,7 @@
         <v>3</v>
       </c>
       <c r="G30" t="s">
-        <v>588</v>
+        <v>562</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -4181,7 +4181,7 @@
         <v>3</v>
       </c>
       <c r="G32" t="s">
-        <v>589</v>
+        <v>563</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -4204,7 +4204,7 @@
         <v>3</v>
       </c>
       <c r="G33" t="s">
-        <v>590</v>
+        <v>564</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -4227,7 +4227,7 @@
         <v>3</v>
       </c>
       <c r="G34" t="s">
-        <v>576</v>
+        <v>550</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -4250,7 +4250,7 @@
         <v>3</v>
       </c>
       <c r="G35" t="s">
-        <v>591</v>
+        <v>565</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -4273,7 +4273,7 @@
         <v>3</v>
       </c>
       <c r="G36" t="s">
-        <v>592</v>
+        <v>566</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -4296,7 +4296,7 @@
         <v>3</v>
       </c>
       <c r="G37" t="s">
-        <v>593</v>
+        <v>567</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -4319,7 +4319,7 @@
         <v>3</v>
       </c>
       <c r="G38" t="s">
-        <v>594</v>
+        <v>568</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -4342,7 +4342,7 @@
         <v>3</v>
       </c>
       <c r="G39" t="s">
-        <v>595</v>
+        <v>569</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -4365,7 +4365,7 @@
         <v>3</v>
       </c>
       <c r="G40" t="s">
-        <v>596</v>
+        <v>570</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -4388,7 +4388,7 @@
         <v>3</v>
       </c>
       <c r="G41" t="s">
-        <v>597</v>
+        <v>571</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -4411,7 +4411,7 @@
         <v>3</v>
       </c>
       <c r="G42" t="s">
-        <v>598</v>
+        <v>572</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -4434,7 +4434,7 @@
         <v>3</v>
       </c>
       <c r="G43" t="s">
-        <v>599</v>
+        <v>573</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -4457,7 +4457,7 @@
         <v>3</v>
       </c>
       <c r="G44" t="s">
-        <v>562</v>
+        <v>536</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
@@ -4480,7 +4480,7 @@
         <v>3</v>
       </c>
       <c r="G45" t="s">
-        <v>600</v>
+        <v>574</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -4503,7 +4503,7 @@
         <v>3</v>
       </c>
       <c r="G46" t="s">
-        <v>601</v>
+        <v>575</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
@@ -4526,7 +4526,7 @@
         <v>3</v>
       </c>
       <c r="G47" t="s">
-        <v>602</v>
+        <v>576</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -4549,7 +4549,7 @@
         <v>3</v>
       </c>
       <c r="G48" t="s">
-        <v>603</v>
+        <v>577</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
@@ -4572,7 +4572,7 @@
         <v>3</v>
       </c>
       <c r="G49" t="s">
-        <v>604</v>
+        <v>578</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
@@ -4595,7 +4595,7 @@
         <v>3</v>
       </c>
       <c r="G50" t="s">
-        <v>605</v>
+        <v>579</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
@@ -4618,7 +4618,7 @@
         <v>3</v>
       </c>
       <c r="G51" t="s">
-        <v>606</v>
+        <v>580</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
@@ -4641,7 +4641,7 @@
         <v>3</v>
       </c>
       <c r="G52" t="s">
-        <v>607</v>
+        <v>581</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
@@ -4687,7 +4687,7 @@
         <v>3</v>
       </c>
       <c r="G54" t="s">
-        <v>608</v>
+        <v>582</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
@@ -4710,7 +4710,7 @@
         <v>3</v>
       </c>
       <c r="G55" t="s">
-        <v>609</v>
+        <v>583</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
@@ -4733,7 +4733,7 @@
         <v>3</v>
       </c>
       <c r="G56" t="s">
-        <v>610</v>
+        <v>584</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
@@ -4756,7 +4756,7 @@
         <v>3</v>
       </c>
       <c r="G57" t="s">
-        <v>611</v>
+        <v>585</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
@@ -4779,7 +4779,7 @@
         <v>3</v>
       </c>
       <c r="G58" t="s">
-        <v>612</v>
+        <v>586</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
@@ -4802,7 +4802,7 @@
         <v>3</v>
       </c>
       <c r="G59" t="s">
-        <v>613</v>
+        <v>587</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
@@ -4825,7 +4825,7 @@
         <v>3</v>
       </c>
       <c r="G60" t="s">
-        <v>614</v>
+        <v>588</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
@@ -4848,7 +4848,7 @@
         <v>3</v>
       </c>
       <c r="G61" t="s">
-        <v>614</v>
+        <v>588</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
@@ -4871,7 +4871,7 @@
         <v>3</v>
       </c>
       <c r="G62" t="s">
-        <v>615</v>
+        <v>589</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
@@ -4894,7 +4894,7 @@
         <v>3</v>
       </c>
       <c r="G63" t="s">
-        <v>569</v>
+        <v>543</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
@@ -4917,7 +4917,7 @@
         <v>3</v>
       </c>
       <c r="G64" t="s">
-        <v>616</v>
+        <v>590</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
@@ -4940,7 +4940,7 @@
         <v>3</v>
       </c>
       <c r="G65" t="s">
-        <v>617</v>
+        <v>591</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
@@ -4963,7 +4963,7 @@
         <v>3</v>
       </c>
       <c r="G66" t="s">
-        <v>618</v>
+        <v>592</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
@@ -4986,7 +4986,7 @@
         <v>3</v>
       </c>
       <c r="G67" t="s">
-        <v>619</v>
+        <v>593</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
@@ -5009,7 +5009,7 @@
         <v>3</v>
       </c>
       <c r="G68" t="s">
-        <v>620</v>
+        <v>594</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
@@ -5032,7 +5032,7 @@
         <v>3</v>
       </c>
       <c r="G69" t="s">
-        <v>621</v>
+        <v>595</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
@@ -5055,7 +5055,7 @@
         <v>3</v>
       </c>
       <c r="G70" t="s">
-        <v>622</v>
+        <v>596</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
@@ -5078,7 +5078,7 @@
         <v>3</v>
       </c>
       <c r="G71" t="s">
-        <v>623</v>
+        <v>597</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
@@ -5101,7 +5101,7 @@
         <v>3</v>
       </c>
       <c r="G72" t="s">
-        <v>624</v>
+        <v>598</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
@@ -5124,7 +5124,7 @@
         <v>3</v>
       </c>
       <c r="G73" t="s">
-        <v>625</v>
+        <v>599</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
@@ -5147,7 +5147,7 @@
         <v>3</v>
       </c>
       <c r="G74" t="s">
-        <v>626</v>
+        <v>600</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
@@ -5170,7 +5170,7 @@
         <v>3</v>
       </c>
       <c r="G75" t="s">
-        <v>627</v>
+        <v>601</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
@@ -5193,7 +5193,7 @@
         <v>3</v>
       </c>
       <c r="G76" t="s">
-        <v>628</v>
+        <v>602</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
@@ -5216,7 +5216,7 @@
         <v>3</v>
       </c>
       <c r="G77" t="s">
-        <v>629</v>
+        <v>603</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
@@ -5239,7 +5239,7 @@
         <v>3</v>
       </c>
       <c r="G78" t="s">
-        <v>630</v>
+        <v>604</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
@@ -5262,7 +5262,7 @@
         <v>3</v>
       </c>
       <c r="G79" t="s">
-        <v>631</v>
+        <v>605</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
@@ -5285,7 +5285,7 @@
         <v>3</v>
       </c>
       <c r="G80" t="s">
-        <v>632</v>
+        <v>606</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
@@ -5308,7 +5308,7 @@
         <v>3</v>
       </c>
       <c r="G81" t="s">
-        <v>587</v>
+        <v>561</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
@@ -5331,7 +5331,7 @@
         <v>3</v>
       </c>
       <c r="G82" t="s">
-        <v>587</v>
+        <v>561</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
@@ -5354,7 +5354,7 @@
         <v>3</v>
       </c>
       <c r="G83" t="s">
-        <v>633</v>
+        <v>607</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
@@ -5377,7 +5377,7 @@
         <v>3</v>
       </c>
       <c r="G84" t="s">
-        <v>634</v>
+        <v>608</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
@@ -5400,7 +5400,7 @@
         <v>3</v>
       </c>
       <c r="G85" t="s">
-        <v>635</v>
+        <v>609</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
@@ -5423,7 +5423,7 @@
         <v>3</v>
       </c>
       <c r="G86" t="s">
-        <v>581</v>
+        <v>555</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
@@ -5446,7 +5446,7 @@
         <v>3</v>
       </c>
       <c r="G87" t="s">
-        <v>636</v>
+        <v>610</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
@@ -5469,7 +5469,7 @@
         <v>3</v>
       </c>
       <c r="G88" t="s">
-        <v>637</v>
+        <v>611</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
@@ -5492,7 +5492,7 @@
         <v>3</v>
       </c>
       <c r="G89" t="s">
-        <v>638</v>
+        <v>612</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
@@ -5515,7 +5515,7 @@
         <v>3</v>
       </c>
       <c r="G90" t="s">
-        <v>639</v>
+        <v>613</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
@@ -5538,7 +5538,7 @@
         <v>3</v>
       </c>
       <c r="G91" t="s">
-        <v>640</v>
+        <v>614</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
@@ -5561,7 +5561,7 @@
         <v>3</v>
       </c>
       <c r="G92" t="s">
-        <v>641</v>
+        <v>615</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
@@ -5584,7 +5584,7 @@
         <v>3</v>
       </c>
       <c r="G93" t="s">
-        <v>642</v>
+        <v>616</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
@@ -5607,7 +5607,7 @@
         <v>3</v>
       </c>
       <c r="G94" t="s">
-        <v>643</v>
+        <v>617</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
@@ -5630,7 +5630,7 @@
         <v>3</v>
       </c>
       <c r="G95" t="s">
-        <v>644</v>
+        <v>618</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
@@ -5653,7 +5653,7 @@
         <v>3</v>
       </c>
       <c r="G96" t="s">
-        <v>578</v>
+        <v>552</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
@@ -5676,7 +5676,7 @@
         <v>3</v>
       </c>
       <c r="G97" t="s">
-        <v>645</v>
+        <v>619</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
@@ -5699,7 +5699,7 @@
         <v>3</v>
       </c>
       <c r="G98" t="s">
-        <v>646</v>
+        <v>620</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
@@ -5722,7 +5722,7 @@
         <v>3</v>
       </c>
       <c r="G99" t="s">
-        <v>647</v>
+        <v>621</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
@@ -5745,7 +5745,7 @@
         <v>3</v>
       </c>
       <c r="G100" t="s">
-        <v>648</v>
+        <v>622</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
@@ -5768,7 +5768,7 @@
         <v>3</v>
       </c>
       <c r="G101" t="s">
-        <v>649</v>
+        <v>623</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
@@ -5791,7 +5791,7 @@
         <v>3</v>
       </c>
       <c r="G102" t="s">
-        <v>650</v>
+        <v>624</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
@@ -5814,7 +5814,7 @@
         <v>3</v>
       </c>
       <c r="G103" t="s">
-        <v>651</v>
+        <v>625</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
@@ -5837,7 +5837,7 @@
         <v>3</v>
       </c>
       <c r="G104" t="s">
-        <v>652</v>
+        <v>626</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.3">
@@ -5860,7 +5860,7 @@
         <v>3</v>
       </c>
       <c r="G105" t="s">
-        <v>653</v>
+        <v>627</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
@@ -5883,7 +5883,7 @@
         <v>3</v>
       </c>
       <c r="G106" t="s">
-        <v>654</v>
+        <v>628</v>
       </c>
     </row>
   </sheetData>
@@ -5896,8 +5896,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5911,19 +5911,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>434</v>
+        <v>419</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>435</v>
+        <v>420</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -6008,7 +6008,7 @@
         <v>313</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>314</v>
+        <v>629</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -6016,13 +6016,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>316</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>317</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>301</v>
@@ -6033,16 +6033,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>320</v>
-      </c>
       <c r="E8" s="2" t="s">
-        <v>321</v>
+        <v>630</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -6050,16 +6050,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>324</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>325</v>
+        <v>631</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -6067,16 +6067,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>326</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -6084,16 +6084,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>330</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -6101,16 +6101,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>334</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>336</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -6118,16 +6118,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>341</v>
+        <v>632</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -6135,16 +6135,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>344</v>
+        <v>633</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -6152,13 +6152,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>301</v>
@@ -6172,13 +6172,13 @@
         <v>298</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>350</v>
+        <v>634</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -6186,16 +6186,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>350</v>
+        <v>634</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -6203,13 +6203,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>301</v>
@@ -6220,13 +6220,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>301</v>
@@ -6237,16 +6237,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -6254,16 +6254,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -6271,16 +6271,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -6288,16 +6288,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -6305,16 +6305,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -6322,13 +6322,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>301</v>
@@ -6339,16 +6339,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>383</v>
+        <v>635</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -6356,16 +6356,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>387</v>
+        <v>636</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -6373,16 +6373,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>387</v>
+        <v>636</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -6390,16 +6390,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>394</v>
+        <v>637</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -6407,16 +6407,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>398</v>
+        <v>638</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -6424,16 +6424,16 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>402</v>
+        <v>639</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -6441,16 +6441,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>403</v>
+        <v>392</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>404</v>
+        <v>393</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>405</v>
+        <v>394</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>406</v>
+        <v>640</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -6458,13 +6458,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>408</v>
+        <v>396</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>409</v>
+        <v>397</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>301</v>
@@ -6475,16 +6475,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>410</v>
+        <v>398</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>411</v>
+        <v>399</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>413</v>
+        <v>641</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -6492,16 +6492,16 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>414</v>
+        <v>401</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>415</v>
+        <v>402</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>416</v>
+        <v>403</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>417</v>
+        <v>642</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -6509,16 +6509,16 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>418</v>
+        <v>404</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>419</v>
+        <v>405</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>421</v>
+        <v>643</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -6526,16 +6526,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>422</v>
+        <v>407</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>423</v>
+        <v>408</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>413</v>
+        <v>641</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -6543,16 +6543,16 @@
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>473</v>
+        <v>458</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>474</v>
+        <v>459</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>472</v>
+        <v>457</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>475</v>
+        <v>644</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -6560,16 +6560,16 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>486</v>
+        <v>469</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>485</v>
+        <v>468</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>483</v>
+        <v>467</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>484</v>
+        <v>645</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -6577,16 +6577,16 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>489</v>
+        <v>471</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>490</v>
+        <v>472</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>487</v>
+        <v>470</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>488</v>
+        <v>646</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -6594,16 +6594,16 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>494</v>
+        <v>475</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>493</v>
+        <v>474</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>491</v>
+        <v>473</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>492</v>
+        <v>647</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -6611,16 +6611,16 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>494</v>
+        <v>475</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>496</v>
+        <v>477</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>495</v>
+        <v>476</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>497</v>
+        <v>648</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -6628,16 +6628,16 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>499</v>
+        <v>479</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>500</v>
+        <v>480</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>498</v>
+        <v>478</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>501</v>
+        <v>649</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -6645,16 +6645,16 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>506</v>
+        <v>485</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>502</v>
+        <v>481</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>325</v>
+        <v>631</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -6662,16 +6662,16 @@
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>503</v>
+        <v>482</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>505</v>
+        <v>484</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>504</v>
+        <v>483</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -6679,16 +6679,16 @@
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>509</v>
+        <v>488</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>510</v>
+        <v>489</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>507</v>
+        <v>486</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>508</v>
+        <v>487</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -6696,16 +6696,16 @@
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>513</v>
+        <v>492</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>512</v>
+        <v>491</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>511</v>
+        <v>490</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>514</v>
+        <v>493</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -6713,16 +6713,16 @@
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>527</v>
+        <v>506</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>528</v>
+        <v>507</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>525</v>
+        <v>504</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>526</v>
+        <v>505</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -6730,16 +6730,16 @@
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>532</v>
+        <v>510</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>531</v>
+        <v>509</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>529</v>
+        <v>508</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>530</v>
+        <v>650</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -6747,16 +6747,16 @@
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>533</v>
+        <v>511</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>534</v>
+        <v>512</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>535</v>
+        <v>513</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>536</v>
+        <v>651</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -6764,16 +6764,16 @@
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>538</v>
+        <v>515</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>539</v>
+        <v>516</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>537</v>
+        <v>514</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>501</v>
+        <v>649</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -6781,16 +6781,16 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>540</v>
+        <v>517</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>541</v>
+        <v>518</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>542</v>
+        <v>519</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>543</v>
+        <v>652</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -6798,16 +6798,16 @@
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>544</v>
+        <v>520</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>545</v>
+        <v>521</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>546</v>
+        <v>522</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>547</v>
+        <v>523</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -6815,16 +6815,16 @@
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>548</v>
+        <v>524</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>549</v>
+        <v>525</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>550</v>
+        <v>526</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>551</v>
+        <v>653</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -6832,16 +6832,16 @@
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>552</v>
+        <v>527</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>553</v>
+        <v>528</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>554</v>
+        <v>529</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>555</v>
+        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -6917,19 +6917,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>436</v>
+        <v>421</v>
       </c>
       <c r="B1" t="s">
-        <v>438</v>
+        <v>423</v>
       </c>
       <c r="C1" t="s">
-        <v>426</v>
+        <v>411</v>
       </c>
       <c r="D1" t="s">
-        <v>439</v>
+        <v>424</v>
       </c>
       <c r="E1" t="s">
-        <v>425</v>
+        <v>410</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -6940,10 +6940,10 @@
         <v>43737</v>
       </c>
       <c r="C2" t="s">
-        <v>442</v>
+        <v>427</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>467</v>
+        <v>452</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -6954,10 +6954,10 @@
         <v>43862</v>
       </c>
       <c r="C3" t="s">
-        <v>443</v>
+        <v>428</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>468</v>
+        <v>453</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -6968,10 +6968,10 @@
         <v>43863</v>
       </c>
       <c r="C4" t="s">
-        <v>444</v>
+        <v>429</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>469</v>
+        <v>454</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -6982,10 +6982,10 @@
         <v>43870</v>
       </c>
       <c r="C5" t="s">
-        <v>445</v>
+        <v>430</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>470</v>
+        <v>455</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -6996,10 +6996,10 @@
         <v>43893</v>
       </c>
       <c r="C6" t="s">
-        <v>446</v>
+        <v>431</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>471</v>
+        <v>456</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -7007,13 +7007,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>516</v>
+        <v>495</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>517</v>
+        <v>496</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>515</v>
+        <v>494</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -7021,13 +7021,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>516</v>
+        <v>495</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>519</v>
+        <v>498</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>518</v>
+        <v>497</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -7035,13 +7035,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>516</v>
+        <v>495</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>520</v>
+        <v>499</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>521</v>
+        <v>500</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -7049,13 +7049,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>516</v>
+        <v>495</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>523</v>
+        <v>502</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>524</v>
+        <v>503</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -7063,13 +7063,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>516</v>
+        <v>495</v>
       </c>
       <c r="C11" t="s">
-        <v>522</v>
+        <v>501</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>556</v>
+        <v>530</v>
       </c>
     </row>
   </sheetData>
@@ -7094,25 +7094,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>437</v>
+        <v>422</v>
       </c>
       <c r="B1" t="s">
-        <v>440</v>
+        <v>425</v>
       </c>
       <c r="C1" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
       <c r="D1" t="s">
-        <v>441</v>
+        <v>426</v>
       </c>
       <c r="E1" t="s">
-        <v>434</v>
+        <v>419</v>
       </c>
       <c r="F1" t="s">
-        <v>426</v>
+        <v>411</v>
       </c>
       <c r="G1" t="s">
-        <v>425</v>
+        <v>410</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -7120,17 +7120,17 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>458</v>
+        <v>443</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>455</v>
+        <v>440</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>451</v>
+        <v>436</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="6" t="s">
-        <v>450</v>
+        <v>435</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -7138,17 +7138,17 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>459</v>
+        <v>444</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>456</v>
+        <v>441</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>452</v>
+        <v>437</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="6" t="s">
-        <v>449</v>
+        <v>434</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -7156,17 +7156,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>461</v>
+        <v>446</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>457</v>
+        <v>442</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>452</v>
+        <v>437</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="6" t="s">
-        <v>448</v>
+        <v>433</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="19.2" x14ac:dyDescent="0.45">
@@ -7174,19 +7174,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>460</v>
+        <v>445</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>454</v>
+        <v>439</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>451</v>
+        <v>436</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>453</v>
+        <v>438</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>447</v>
+        <v>432</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -7194,19 +7194,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>465</v>
+        <v>450</v>
       </c>
       <c r="C6" t="s">
-        <v>479</v>
+        <v>463</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>462</v>
+        <v>447</v>
       </c>
       <c r="E6" t="s">
-        <v>463</v>
+        <v>448</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>464</v>
+        <v>449</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -7214,16 +7214,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>477</v>
+        <v>461</v>
       </c>
       <c r="C7" t="s">
-        <v>476</v>
+        <v>460</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>452</v>
+        <v>437</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>478</v>
+        <v>462</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -7231,16 +7231,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>481</v>
+        <v>465</v>
       </c>
       <c r="C8" t="s">
-        <v>482</v>
+        <v>466</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>452</v>
+        <v>437</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>480</v>
+        <v>464</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -7734,16 +7734,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>466</v>
+        <v>451</v>
       </c>
       <c r="B1" t="s">
-        <v>438</v>
+        <v>423</v>
       </c>
       <c r="C1" t="s">
-        <v>439</v>
+        <v>424</v>
       </c>
       <c r="D1" t="s">
-        <v>425</v>
+        <v>410</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Push before publishing test
</commit_message>
<xml_diff>
--- a/MySite/blog/static/websiteDB.xlsx
+++ b/MySite/blog/static/websiteDB.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\users\15314\source\repos\mysite\mysite\blog\static\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15314\source\repos\MySite\MySite\blog\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7658ECD6-80A7-4CC9-A9F3-774CDCB478FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3D782E-37B2-4EEB-8B1F-812FB64C81BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{E658BFBE-975E-47B3-8C51-826238D4C145}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{E658BFBE-975E-47B3-8C51-826238D4C145}"/>
   </bookViews>
   <sheets>
     <sheet name="Posts" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="658">
   <si>
     <t>50 Economics Classics: Your shortcut to the most important ideas on capitalism; finance; and the global economy</t>
   </si>
@@ -2309,6 +2309,15 @@
   </si>
   <si>
     <t>Finance, blog, research</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/c/Coreyms/playlists</t>
+  </si>
+  <si>
+    <t>Pretty awesome python videos</t>
+  </si>
+  <si>
+    <t>Corey Schafer</t>
   </si>
 </sst>
 </file>
@@ -5894,10 +5903,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87CB60D4-93F8-4068-A531-8A581990591B}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6842,6 +6851,23 @@
       </c>
       <c r="E55" s="2" t="s">
         <v>654</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>657</v>
+      </c>
+      <c r="C56" t="s">
+        <v>656</v>
+      </c>
+      <c r="D56" s="12" t="s">
+        <v>655</v>
+      </c>
+      <c r="E56" t="s">
+        <v>653</v>
       </c>
     </row>
   </sheetData>
@@ -6894,9 +6920,10 @@
     <hyperlink ref="D54" r:id="rId46" xr:uid="{C1527F8B-F94B-408C-BBDD-285C6454C001}"/>
     <hyperlink ref="D55" r:id="rId47" xr:uid="{67B808D3-9D70-472B-9EB3-B72ADFBE8974}"/>
     <hyperlink ref="D2" r:id="rId48" xr:uid="{D694D7D7-671A-4CC8-9A80-0D38A5951FA4}"/>
+    <hyperlink ref="D56" r:id="rId49" xr:uid="{E4C6082D-26C3-4279-836E-50F2458A258E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId49"/>
+  <pageSetup orientation="portrait" r:id="rId50"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added export databases to csv files functionality
</commit_message>
<xml_diff>
--- a/MySite/blog/static/websiteDB.xlsx
+++ b/MySite/blog/static/websiteDB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15314\source\repos\MySite\MySite\blog\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3D782E-37B2-4EEB-8B1F-812FB64C81BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074F25A9-D2E0-4C29-989B-63A9CCDBD304}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{E658BFBE-975E-47B3-8C51-826238D4C145}"/>
+    <workbookView xWindow="13536" yWindow="7476" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{E658BFBE-975E-47B3-8C51-826238D4C145}"/>
   </bookViews>
   <sheets>
     <sheet name="Posts" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="658">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="662">
   <si>
     <t>50 Economics Classics: Your shortcut to the most important ideas on capitalism; finance; and the global economy</t>
   </si>
@@ -2318,6 +2318,18 @@
   </si>
   <si>
     <t>Corey Schafer</t>
+  </si>
+  <si>
+    <t>https://www.pythoncheatsheet.org/</t>
+  </si>
+  <si>
+    <t>Python, Cheatsheet</t>
+  </si>
+  <si>
+    <t>Python Cheatsheet</t>
+  </si>
+  <si>
+    <t>Amazing cheatsheets or python reference source</t>
   </si>
 </sst>
 </file>
@@ -5903,10 +5915,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87CB60D4-93F8-4068-A531-8A581990591B}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6868,6 +6880,23 @@
       </c>
       <c r="E56" t="s">
         <v>653</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>660</v>
+      </c>
+      <c r="C57" t="s">
+        <v>661</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>658</v>
+      </c>
+      <c r="E57" t="s">
+        <v>659</v>
       </c>
     </row>
   </sheetData>
@@ -6921,9 +6950,10 @@
     <hyperlink ref="D55" r:id="rId47" xr:uid="{67B808D3-9D70-472B-9EB3-B72ADFBE8974}"/>
     <hyperlink ref="D2" r:id="rId48" xr:uid="{D694D7D7-671A-4CC8-9A80-0D38A5951FA4}"/>
     <hyperlink ref="D56" r:id="rId49" xr:uid="{E4C6082D-26C3-4279-836E-50F2458A258E}"/>
+    <hyperlink ref="D57" r:id="rId50" xr:uid="{74793D15-BD17-4399-BB65-BE5CBEAE0A9F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId50"/>
+  <pageSetup orientation="portrait" r:id="rId51"/>
 </worksheet>
 </file>
 

</xml_diff>